<commit_message>
set grids to use virtual grids fix all shared settings
</commit_message>
<xml_diff>
--- a/Grid changes tracking.xlsx
+++ b/Grid changes tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\GitRepo\FTAnalyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA1A6C3-9B98-4007-B42D-6D281A6B0CBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA64B32A-56F9-4C5B-932D-780E0FAD7077}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20666" yWindow="4483" windowWidth="11768" windowHeight="13054" xr2:uid="{E7A2A291-F5C5-4BCB-98ED-BB33B652FEEE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
   <si>
     <t>Grid Name</t>
   </si>
@@ -103,6 +103,24 @@
   </si>
   <si>
     <t>yes (some tweaks)</t>
+  </si>
+  <si>
+    <t>data bindings to nameof</t>
+  </si>
+  <si>
+    <t>databound eventhandler calling databound items</t>
+  </si>
+  <si>
+    <t>Event Handler Grids</t>
+  </si>
+  <si>
+    <t>census</t>
+  </si>
+  <si>
+    <t>BMDReportSheet</t>
+  </si>
+  <si>
+    <t>Still to Consider</t>
   </si>
 </sst>
 </file>
@@ -146,9 +164,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF614486-A5DF-4326-BC36-46922F33C0A8}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -474,20 +495,31 @@
     <col min="1" max="1" width="11.765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.4609375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.765625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -498,7 +530,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -509,7 +541,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -520,7 +552,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -531,7 +563,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -542,7 +574,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -553,7 +585,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -564,7 +596,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -575,7 +607,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -586,7 +618,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -597,7 +629,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -608,7 +640,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -619,7 +651,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -630,7 +662,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -641,7 +673,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -680,6 +712,24 @@
       </c>
       <c r="B19" t="s">
         <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A21" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>